<commit_message>
Added new list arrow performance tests versus linq queries and loop-based functions
</commit_message>
<xml_diff>
--- a/Evaluation graphs.xlsx
+++ b/Evaluation graphs.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="5190" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="5190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Identity chain length" sheetId="1" r:id="rId1"/>
     <sheet name="Old arrow-func-function test" sheetId="2" r:id="rId2"/>
     <sheet name="Arrow-func-function test" sheetId="3" r:id="rId3"/>
+    <sheet name="List arrow test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>RunArrow</t>
   </si>
@@ -37,6 +38,39 @@
   </si>
   <si>
     <t>Arctan</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>OrderByThenMap</t>
+  </si>
+  <si>
+    <t>Foldl</t>
+  </si>
+  <si>
+    <t>Linq-based function</t>
+  </si>
+  <si>
+    <t>Loop-based function</t>
+  </si>
+  <si>
+    <t>Makes sense: Linq is slower than loop-based, and arrows use loop-based but with arrow overhead so they come second</t>
+  </si>
+  <si>
+    <t>Would be more even but for the complexity of arrow concatentation discussed elsewhere (does more damage here as the Linq expressions are being ToList()-ed every time)</t>
+  </si>
+  <si>
+    <t>Arrows win! Functions are painful for this, Linq has slow-ish builtin support and the arrows got lucky (they implement it in a reeeeasonably similar way to the function's way so shouldn't really be much quicker)</t>
   </si>
 </sst>
 </file>
@@ -127,84 +161,6 @@
             <c:errBarType val="both"/>
             <c:errValType val="stdErr"/>
             <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Identity chain length'!$D$2:$D$21</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="20"/>
-                  <c:pt idx="0">
-                    <c:v>10.920070000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>9.98893784163762</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>18.1926865309552</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>12.958416292390799</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>11.674045879882399</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>15.677906467704799</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>20.28013</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>7.6424569872783703</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>9.3600600000000007</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>15.677906467704799</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>10.920070000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>15.2849139745567</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>17.16011</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>10.920070000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>18.524092399200001</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>15.2849139745567</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>12.577202709923201</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>15.2849139745567</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>22.116958905331</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>23.1912159065044</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numLit>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numLit>
-            </c:minus>
           </c:errBars>
           <c:val>
             <c:numRef>
@@ -287,11 +243,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105257216"/>
-        <c:axId val="105300736"/>
+        <c:axId val="91694592"/>
+        <c:axId val="91696512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105257216"/>
+        <c:axId val="91694592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +275,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105300736"/>
+        <c:crossAx val="91696512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -327,7 +283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105300736"/>
+        <c:axId val="91696512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -363,7 +319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105257216"/>
+        <c:crossAx val="91694592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -595,11 +551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40876288"/>
-        <c:axId val="40935424"/>
+        <c:axId val="56075776"/>
+        <c:axId val="56077312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40876288"/>
+        <c:axId val="56075776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40935424"/>
+        <c:crossAx val="56077312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -616,7 +572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40935424"/>
+        <c:axId val="56077312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,14 +583,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40876288"/>
+        <c:crossAx val="56075776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -679,7 +634,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RunArrow</c:v>
+                  <c:v>Arrow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -736,7 +691,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RunFunc</c:v>
+                  <c:v>Func</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -793,7 +748,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RunFunction</c:v>
+                  <c:v>Function</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -850,11 +805,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43868160"/>
-        <c:axId val="43870464"/>
+        <c:axId val="91730688"/>
+        <c:axId val="91732224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43868160"/>
+        <c:axId val="91730688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43870464"/>
+        <c:crossAx val="91732224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -871,18 +826,301 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43870464"/>
+        <c:axId val="91732224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time to execute all</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> iterations </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43868160"/>
+        <c:crossAx val="91730688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'List arrow test'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Arrow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'List arrow test'!$B$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Filter</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OrderByThenMap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Foldl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'List arrow test'!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>542.88347999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1154.4074000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>658.32421999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'List arrow test'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linq-based function</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'List arrow test'!$B$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Filter</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OrderByThenMap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Foldl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'List arrow test'!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>624.00400000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>789.36505999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>712.92457000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'List arrow test'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loop-based function</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'List arrow test'!$B$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Filter</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OrderByThenMap</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Foldl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'List arrow test'!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>486.72311999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>755.04484000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>728.52467000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="95284224"/>
+        <c:axId val="95421952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="95284224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95421952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95421952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time to execute all iterations (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95284224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -988,6 +1226,41 @@
       <xdr:colOff>266699</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1298,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1649,25 +1922,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -1724,6 +1998,91 @@
       </c>
       <c r="E6">
         <v>586.56376</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>542.88347999999996</v>
+      </c>
+      <c r="D3">
+        <v>624.00400000000002</v>
+      </c>
+      <c r="E3">
+        <v>486.72311999999999</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>1154.4074000000001</v>
+      </c>
+      <c r="D4">
+        <v>789.36505999999997</v>
+      </c>
+      <c r="E4">
+        <v>755.04484000000002</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>658.32421999999997</v>
+      </c>
+      <c r="D5">
+        <v>712.92457000000002</v>
+      </c>
+      <c r="E5">
+        <v>728.52467000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>